<commit_message>
Agregada la unidad aritmetica
</commit_message>
<xml_diff>
--- a/Documentacion/TABLAVERDAD_ALU.xlsx
+++ b/Documentacion/TABLAVERDAD_ALU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Isaac Porras\Semestre 7\Taller de Diseño Analogico\ALU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skryf\Documents\Taller de Diseno Digital\Laboratorio 3\TallerDiseno-LAB3\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1615B20A-C7B4-4B09-9A45-3AA5A849A67A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FBB8E5-580A-42D1-9301-7DB109B9CBD0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AF67AB85-41AA-4EE4-A15A-BA1E3D722A48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF67AB85-41AA-4EE4-A15A-BA1E3D722A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>ALU Control</t>
   </si>
@@ -57,12 +57,6 @@
     <t>AND</t>
   </si>
   <si>
-    <t>LEFT SHIFT</t>
-  </si>
-  <si>
-    <t>RIGHT SHIFT</t>
-  </si>
-  <si>
     <t>NOT</t>
   </si>
   <si>
@@ -73,6 +67,21 @@
   </si>
   <si>
     <t>Restador</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A RIGHT SHIFT</t>
+  </si>
+  <si>
+    <t>B LEFT SHIFT</t>
+  </si>
+  <si>
+    <t>A LEFT SHIFT</t>
+  </si>
+  <si>
+    <t>B RIGHT SHIFT</t>
+  </si>
+  <si>
+    <t>A RIGHT SHIFT</t>
   </si>
 </sst>
 </file>
@@ -155,9 +164,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -165,6 +171,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -185,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,343 +493,346 @@
   <dimension ref="A5:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>0</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="4" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>0</v>
-      </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>0</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>0</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>